<commit_message>
update marging en spaces
</commit_message>
<xml_diff>
--- a/build/downloads/D&B TEMPLATE1.xlsx
+++ b/build/downloads/D&B TEMPLATE1.xlsx
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="13">
   <si>
     <t>ITEM</t>
   </si>
@@ -108,82 +108,7 @@
     <t>NEXT DUE</t>
   </si>
   <si>
-    <t>dent</t>
-  </si>
-  <si>
-    <t>dent on frame 3</t>
-  </si>
-  <si>
-    <t>fr 3 - 4</t>
-  </si>
-  <si>
-    <t>str 3-6</t>
-  </si>
-  <si>
-    <t>nacelle</t>
-  </si>
-  <si>
-    <t>4*5*6</t>
-  </si>
-  <si>
-    <t>SRM 5724156</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>OK</t>
-  </si>
-  <si>
-    <t>gerg</t>
-  </si>
-  <si>
-    <t>reg</t>
-  </si>
-  <si>
-    <t>gerer</t>
-  </si>
-  <si>
-    <t>erg</t>
-  </si>
-  <si>
-    <t>egr</t>
-  </si>
-  <si>
-    <t>eg</t>
-  </si>
-  <si>
-    <t>ñkernnv</t>
-  </si>
-  <si>
-    <t>ññernb</t>
-  </si>
-  <si>
-    <t>vnwñrnv</t>
-  </si>
-  <si>
-    <t>ñwrng</t>
-  </si>
-  <si>
-    <t>ñwren</t>
-  </si>
-  <si>
-    <t>vñrewn</t>
-  </si>
-  <si>
-    <t>vñwrlnv</t>
-  </si>
-  <si>
-    <t>vñrlnv</t>
-  </si>
-  <si>
-    <t>vñrln</t>
-  </si>
-  <si>
-    <t>vñwlne</t>
-  </si>
-  <si>
-    <t>vñwlen</t>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -191,9 +116,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
@@ -241,14 +166,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -304,21 +221,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -334,18 +236,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -359,6 +262,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -382,6 +292,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -433,19 +358,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -469,19 +388,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -499,7 +406,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -511,7 +436,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -523,19 +454,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -547,25 +466,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -589,19 +508,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -726,15 +651,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -752,10 +668,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -823,151 +737,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2038,7 +1963,7 @@
   <dimension ref="A2:Z988"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:R7"/>
+      <selection activeCell="B4" sqref="B4:R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
@@ -2114,40 +2039,40 @@
         <v>12</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="8" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="K3" s="19"/>
       <c r="L3" s="6"/>
       <c r="M3" s="8" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="N3" s="6"/>
       <c r="O3" s="8" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="P3" s="6"/>
       <c r="Q3" s="4" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="S3" s="21"/>
       <c r="T3" s="21"/>
@@ -2162,44 +2087,44 @@
       <c r="A4" s="9">
         <v>2</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>21</v>
+      <c r="B4" s="4" t="s">
+        <v>12</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>22</v>
+      <c r="C4" s="5" t="s">
+        <v>12</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="9" t="s">
-        <v>23</v>
+      <c r="D4" s="6"/>
+      <c r="E4" s="7" t="s">
+        <v>12</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>24</v>
+      <c r="F4" s="7" t="s">
+        <v>12</v>
       </c>
-      <c r="G4" s="9" t="s">
-        <v>24</v>
+      <c r="G4" s="7" t="s">
+        <v>12</v>
       </c>
-      <c r="H4" s="12" t="s">
-        <v>25</v>
+      <c r="H4" s="8" t="s">
+        <v>12</v>
       </c>
-      <c r="I4" s="11"/>
-      <c r="J4" s="12" t="s">
-        <v>26</v>
+      <c r="I4" s="6"/>
+      <c r="J4" s="8" t="s">
+        <v>12</v>
       </c>
-      <c r="K4" s="20"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="12" t="s">
-        <v>25</v>
+      <c r="K4" s="19"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="8" t="s">
+        <v>12</v>
       </c>
-      <c r="N4" s="11"/>
-      <c r="O4" s="12" t="s">
-        <v>25</v>
+      <c r="N4" s="6"/>
+      <c r="O4" s="8" t="s">
+        <v>12</v>
       </c>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="9" t="s">
-        <v>25</v>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="4" t="s">
+        <v>12</v>
       </c>
-      <c r="R4" s="9" t="s">
-        <v>25</v>
+      <c r="R4" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="S4" s="21"/>
       <c r="T4" s="21"/>
@@ -2214,44 +2139,44 @@
       <c r="A5" s="9">
         <v>3</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>27</v>
+      <c r="B5" s="4" t="s">
+        <v>12</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>28</v>
+      <c r="C5" s="5" t="s">
+        <v>12</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="9" t="s">
-        <v>29</v>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7" t="s">
+        <v>12</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>30</v>
+      <c r="F5" s="7" t="s">
+        <v>12</v>
       </c>
-      <c r="G5" s="9" t="s">
-        <v>31</v>
+      <c r="G5" s="7" t="s">
+        <v>12</v>
       </c>
-      <c r="H5" s="12" t="s">
-        <v>32</v>
+      <c r="H5" s="8" t="s">
+        <v>12</v>
       </c>
-      <c r="I5" s="11"/>
-      <c r="J5" s="12" t="s">
-        <v>33</v>
+      <c r="I5" s="6"/>
+      <c r="J5" s="8" t="s">
+        <v>12</v>
       </c>
-      <c r="K5" s="20"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="12" t="s">
-        <v>34</v>
+      <c r="K5" s="19"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="8" t="s">
+        <v>12</v>
       </c>
-      <c r="N5" s="11"/>
-      <c r="O5" s="12" t="s">
-        <v>35</v>
+      <c r="N5" s="6"/>
+      <c r="O5" s="8" t="s">
+        <v>12</v>
       </c>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="9" t="s">
-        <v>36</v>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="4" t="s">
+        <v>12</v>
       </c>
-      <c r="R5" s="9" t="s">
-        <v>37</v>
+      <c r="R5" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="S5" s="21"/>
       <c r="T5" s="21"/>
@@ -2270,40 +2195,40 @@
         <v>12</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="8" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="K6" s="19"/>
       <c r="L6" s="6"/>
       <c r="M6" s="8" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="N6" s="6"/>
       <c r="O6" s="8" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="P6" s="6"/>
       <c r="Q6" s="4" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="S6" s="21"/>
       <c r="T6" s="21"/>
@@ -2318,44 +2243,44 @@
       <c r="A7" s="9">
         <v>5</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>21</v>
+      <c r="B7" s="4" t="s">
+        <v>12</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>22</v>
+      <c r="C7" s="5" t="s">
+        <v>12</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="9" t="s">
-        <v>23</v>
+      <c r="D7" s="6"/>
+      <c r="E7" s="7" t="s">
+        <v>12</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>24</v>
+      <c r="F7" s="7" t="s">
+        <v>12</v>
       </c>
-      <c r="G7" s="9" t="s">
-        <v>24</v>
+      <c r="G7" s="7" t="s">
+        <v>12</v>
       </c>
-      <c r="H7" s="12" t="s">
-        <v>25</v>
+      <c r="H7" s="8" t="s">
+        <v>12</v>
       </c>
-      <c r="I7" s="11"/>
-      <c r="J7" s="12" t="s">
-        <v>26</v>
+      <c r="I7" s="6"/>
+      <c r="J7" s="8" t="s">
+        <v>12</v>
       </c>
-      <c r="K7" s="20"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="12" t="s">
-        <v>25</v>
+      <c r="K7" s="19"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="8" t="s">
+        <v>12</v>
       </c>
-      <c r="N7" s="11"/>
-      <c r="O7" s="12" t="s">
-        <v>25</v>
+      <c r="N7" s="6"/>
+      <c r="O7" s="8" t="s">
+        <v>12</v>
       </c>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="9" t="s">
-        <v>25</v>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="4" t="s">
+        <v>12</v>
       </c>
-      <c r="R7" s="9" t="s">
-        <v>25</v>
+      <c r="R7" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="S7" s="21"/>
       <c r="T7" s="21"/>
@@ -2367,24 +2292,48 @@
       <c r="Z7" s="21"/>
     </row>
     <row r="8" customHeight="1" spans="1:26">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="9"/>
+      <c r="A8" s="9">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="19"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="N8" s="6"/>
+      <c r="O8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="S8" s="21"/>
       <c r="T8" s="21"/>
       <c r="U8" s="21"/>
@@ -2395,24 +2344,48 @@
       <c r="Z8" s="21"/>
     </row>
     <row r="9" customHeight="1" spans="1:26">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9"/>
+      <c r="A9" s="9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" s="19"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="N9" s="6"/>
+      <c r="O9" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="S9" s="21"/>
       <c r="T9" s="21"/>
       <c r="U9" s="21"/>
@@ -2423,24 +2396,48 @@
       <c r="Z9" s="21"/>
     </row>
     <row r="10" customHeight="1" spans="1:26">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
+      <c r="A10" s="9">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K10" s="19"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="N10" s="6"/>
+      <c r="O10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="R10" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="S10" s="21"/>
       <c r="T10" s="21"/>
       <c r="U10" s="21"/>
@@ -2451,24 +2448,48 @@
       <c r="Z10" s="21"/>
     </row>
     <row r="11" customHeight="1" spans="1:26">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9"/>
+      <c r="A11" s="9">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" s="19"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="N11" s="6"/>
+      <c r="O11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="S11" s="21"/>
       <c r="T11" s="21"/>
       <c r="U11" s="21"/>
@@ -2479,24 +2500,48 @@
       <c r="Z11" s="21"/>
     </row>
     <row r="12" customHeight="1" spans="1:26">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
+      <c r="A12" s="9">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="J12" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K12" s="19"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="N12" s="6"/>
+      <c r="O12" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="R12" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="S12" s="21"/>
       <c r="T12" s="21"/>
       <c r="U12" s="21"/>

</xml_diff>